<commit_message>
Carol mudou uma unidade
</commit_message>
<xml_diff>
--- a/report/centros_de_custo.xlsx
+++ b/report/centros_de_custo.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <si>
     <t xml:space="preserve">CF José Mauro Ceratti Lopes - GDRES</t>
   </si>
@@ -300,6 +300,9 @@
   </si>
   <si>
     <t xml:space="preserve">US Rincão - GDGCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US Rubem Berta - GDNEB</t>
   </si>
   <si>
     <t xml:space="preserve">US Safira Nova - GDLN</t>
@@ -735,7 +738,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>